<commit_message>
login and billing address excel
</commit_message>
<xml_diff>
--- a/resources/excel.xlsx
+++ b/resources/excel.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kowshik.saha\IdeaProjects\Magento\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42471877-0EAE-498E-9E37-FA851CE448B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F13909-B0AA-4FBE-8D32-75C48D25AF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="3540" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>Kowshik001</t>
   </si>
@@ -51,26 +51,112 @@
     <t>password</t>
   </si>
   <si>
-    <t>tESpZHYYYN@yopmail.com</t>
-  </si>
-  <si>
-    <t>JkSvgn5vmA@yopmail.com</t>
-  </si>
-  <si>
-    <t>Saha1</t>
-  </si>
-  <si>
-    <t>FXb6Aq42Od@yopmail.com</t>
-  </si>
-  <si>
-    <t>y6UkB2IBFZ@yopmail.com</t>
+    <t>Kowshik003</t>
+  </si>
+  <si>
+    <t>Kowshik004</t>
+  </si>
+  <si>
+    <t>Kowshik005</t>
+  </si>
+  <si>
+    <t>Kowshik006</t>
+  </si>
+  <si>
+    <t>Kowshik007</t>
+  </si>
+  <si>
+    <t>Kowshik008</t>
+  </si>
+  <si>
+    <t>Kowshik009</t>
+  </si>
+  <si>
+    <t>AfL9Mi57Yw@yopmail.com</t>
+  </si>
+  <si>
+    <t>ZCl1sSTe2j@yopmail.com</t>
+  </si>
+  <si>
+    <t>n7yvUkGcdp@yopmail.com</t>
+  </si>
+  <si>
+    <t>0PrFDdQgYo@yopmail.com</t>
+  </si>
+  <si>
+    <t>tx0pzEeeLb@yopmail.com</t>
+  </si>
+  <si>
+    <t>qxGOhDaHwO@yopmail.com</t>
+  </si>
+  <si>
+    <t>jLiAHhReUZ@yopmail.com</t>
+  </si>
+  <si>
+    <t>UDNjZsbrTl@yopmail.com</t>
+  </si>
+  <si>
+    <t>AYowZ6fZSl@yopmail.com</t>
+  </si>
+  <si>
+    <t>street1</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>telephone</t>
+  </si>
+  <si>
+    <t>Police Plaza - Gulshan 1</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
+  </si>
+  <si>
+    <t>United Stated</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Police Plaza - Gulshan 2</t>
+  </si>
+  <si>
+    <t>Police Plaza - Gulshan 3</t>
+  </si>
+  <si>
+    <t>Police Plaza - Gulshan 4</t>
+  </si>
+  <si>
+    <t>Police Plaza - Gulshan 5</t>
+  </si>
+  <si>
+    <t>Police Plaza - Gulshan 6</t>
+  </si>
+  <si>
+    <t>Police Plaza - Gulshan 7</t>
+  </si>
+  <si>
+    <t>Police Plaza - Gulshan 8</t>
+  </si>
+  <si>
+    <t>Police Plaza - Gulshan 9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,22 +495,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="L10" sqref="A1:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.21875"/>
-    <col min="3" max="3" customWidth="true" width="24.6640625"/>
-    <col min="5" max="5" customWidth="true" width="16.0"/>
-    <col min="6" max="6" customWidth="true" width="12.33203125"/>
-    <col min="10" max="10" customWidth="true" width="18.77734375"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -438,8 +524,26 @@
         <v>4</v>
       </c>
       <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,22 +553,282 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1212</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1">
+        <v>484155411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1213</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1">
+        <v>484155412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1214</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="1">
+        <v>484155413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1215</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="1">
+        <v>484155414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1216</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="1">
+        <v>484155415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1217</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="1">
+        <v>484155416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1218</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="1">
+        <v>484155417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1219</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="1">
+        <v>484155418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1220</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="1">
+        <v>484155419</v>
       </c>
     </row>
   </sheetData>
@@ -475,6 +839,7 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Ksl@123" xr:uid="{3AD81FD9-7F57-4054-9695-C75BBFBEDA7F}"/>
     <hyperlink ref="C3" r:id="rId2" display="Ksl@123" xr:uid="{FC1627EB-DC29-44FD-A724-3FFE2D1E7054}"/>
+    <hyperlink ref="C4:C10" r:id="rId3" display="Ksl@123" xr:uid="{825DAAA0-268D-4118-BC78-18067C5352CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
regex changed to String split-more siimplified
</commit_message>
<xml_diff>
--- a/resources/excel.xlsx
+++ b/resources/excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="177">
   <si>
     <t>Kowshik001</t>
   </si>
@@ -394,6 +394,168 @@
   </si>
   <si>
     <t>AdfWoryCy2@yopmail.com</t>
+  </si>
+  <si>
+    <t>bLX4oRuyt6@yopmail.com</t>
+  </si>
+  <si>
+    <t>ajkVcUnA3c@yopmail.com</t>
+  </si>
+  <si>
+    <t>000022325</t>
+  </si>
+  <si>
+    <t>B0O7pzXjag@yopmail.com</t>
+  </si>
+  <si>
+    <t>qLoEvm8ShY@yopmail.com</t>
+  </si>
+  <si>
+    <t>RbL55XAYfr@yopmail.com</t>
+  </si>
+  <si>
+    <t>ho6NAMDFww@yopmail.com</t>
+  </si>
+  <si>
+    <t>Kc0q59ZkrL@yopmail.com</t>
+  </si>
+  <si>
+    <t>nWA9PRsddq@yopmail.com</t>
+  </si>
+  <si>
+    <t>CUd1zYTA4u@yopmail.com</t>
+  </si>
+  <si>
+    <t>5YA0t6ZpRQ@yopmail.com</t>
+  </si>
+  <si>
+    <t>000022328</t>
+  </si>
+  <si>
+    <t>wIJgv7My3i@yopmail.com</t>
+  </si>
+  <si>
+    <t>ply7cOgbK5@yopmail.com</t>
+  </si>
+  <si>
+    <t>Sw1kS32Cej@yopmail.com</t>
+  </si>
+  <si>
+    <t>mToEey8jli@yopmail.com</t>
+  </si>
+  <si>
+    <t>6PfO0ZZmbX@yopmail.com</t>
+  </si>
+  <si>
+    <t>iDgqkxnLkZ@yopmail.com</t>
+  </si>
+  <si>
+    <t>oXgw88PYnX@yopmail.com</t>
+  </si>
+  <si>
+    <t>KqcB9VVl7G@yopmail.com</t>
+  </si>
+  <si>
+    <t>ZPVmcZEztU@yopmail.com</t>
+  </si>
+  <si>
+    <t>7BUoOLXw9z@yopmail.com</t>
+  </si>
+  <si>
+    <t>aUaXZzNDQQ@yopmail.com</t>
+  </si>
+  <si>
+    <t>qfs1zkKkXn@yopmail.com</t>
+  </si>
+  <si>
+    <t>i5kLv6aFOW@yopmail.com</t>
+  </si>
+  <si>
+    <t>p9SDvZyJuT@yopmail.com</t>
+  </si>
+  <si>
+    <t>CTzQbj4P2k@yopmail.com</t>
+  </si>
+  <si>
+    <t>9IAQzWIG4G@yopmail.com</t>
+  </si>
+  <si>
+    <t>fMSEB1GkMy@yopmail.com</t>
+  </si>
+  <si>
+    <t>EJzl50f6i8@yopmail.com</t>
+  </si>
+  <si>
+    <t>YLIPUwy7e2@yopmail.com</t>
+  </si>
+  <si>
+    <t>rh3gxUualz@yopmail.com</t>
+  </si>
+  <si>
+    <t>mRGCH5WJzt@yopmail.com</t>
+  </si>
+  <si>
+    <t>VV428ZLHTJ@yopmail.com</t>
+  </si>
+  <si>
+    <t>T8OGks7Fzl@yopmail.com</t>
+  </si>
+  <si>
+    <t>cztlymFYvq@yopmail.com</t>
+  </si>
+  <si>
+    <t>CIXumf6Vyq@yopmail.com</t>
+  </si>
+  <si>
+    <t>pLSoWYFoVF@yopmail.com</t>
+  </si>
+  <si>
+    <t>lEkT2T4inP@yopmail.com</t>
+  </si>
+  <si>
+    <t>lEcbQ1JnD0@yopmail.com</t>
+  </si>
+  <si>
+    <t>N7Cj7plAIT@yopmail.com</t>
+  </si>
+  <si>
+    <t>cidnXeGV55@yopmail.com</t>
+  </si>
+  <si>
+    <t>bqSTBH9KWJ@yopmail.com</t>
+  </si>
+  <si>
+    <t>gPNiTIfIHT@yopmail.com</t>
+  </si>
+  <si>
+    <t>cmxn6rxUKl@yopmail.com</t>
+  </si>
+  <si>
+    <t>MZohNx4wOR@yopmail.com</t>
+  </si>
+  <si>
+    <t>000022467</t>
+  </si>
+  <si>
+    <t>y1FPEnFbbv@yopmail.com</t>
+  </si>
+  <si>
+    <t>ScWpszqWgS@yopmail.com</t>
+  </si>
+  <si>
+    <t>l0Vj0fPSqg@yopmail.com</t>
+  </si>
+  <si>
+    <t>qo5cMKWDXp@yopmail.com</t>
+  </si>
+  <si>
+    <t>VpDtUTn6ic@yopmail.com</t>
+  </si>
+  <si>
+    <t>o67iEFMWXU@yopmail.com</t>
+  </si>
+  <si>
+    <t>000022472</t>
   </si>
 </sst>
 </file>
@@ -812,9 +974,7 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>121</v>
-      </c>
+      <c r="D2" s="0"/>
       <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
@@ -842,7 +1002,9 @@
       <c r="N2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="0"/>
+      <c r="O2" t="s" s="0">
+        <v>176</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -855,7 +1017,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>17</v>

</xml_diff>